<commit_message>
Sampling Rate: 19200Hz 状態遷移図更新
</commit_message>
<xml_diff>
--- a/PSoC/I2S_FG_状態遷移図.xlsx
+++ b/PSoC/I2S_FG_状態遷移図.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Rotary Encoder/アッテネート</t>
     <phoneticPr fontId="1"/>
@@ -81,23 +81,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>[*] [#]キー</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[A}キー</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[B]キー</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>LCD オン</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>LCD オフ</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -111,10 +95,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2016.02.28</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>通常モード</t>
     <rPh sb="0" eb="2">
       <t>ツウジョウ</t>
@@ -129,13 +109,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>[波形] / [アッテネート]</t>
-    <rPh sb="1" eb="3">
-      <t>ハケイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>波形選択モード</t>
     <rPh sb="0" eb="2">
       <t>ハケイ</t>
@@ -146,32 +119,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>WAVE? 1:SIN</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:SAW 3:SQR</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>設定モード</t>
-    <rPh sb="0" eb="2">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[電源電圧]</t>
-    <rPh sb="1" eb="5">
-      <t>デ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>cont:[コントラスト]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>※[]内は対応する数値</t>
     <rPh sb="3" eb="4">
       <t>ナイ</t>
@@ -237,7 +184,100 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2016.03.01</t>
+    <t>[*]キー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[#]キー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[#]キー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[A}キー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[B]キー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LCD オフ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（保留）</t>
+    <rPh sb="1" eb="3">
+      <t>ホリュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2016.03.27</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[波形]  [アッテネート]</t>
+    <rPh sb="1" eb="3">
+      <t>ハケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>WAV:[波形]</t>
+    <rPh sb="5" eb="7">
+      <t>ハケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ATT:[減衰値]</t>
+    <rPh sb="5" eb="7">
+      <t>ゲンスイ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>コントラスト設定モード</t>
+    <rPh sb="6" eb="8">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CONT:[コントラスト]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>状態表示モード</t>
+    <rPh sb="0" eb="2">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[電源電圧]mV</t>
+    <rPh sb="1" eb="3">
+      <t>デンゲン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>デンアツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[ダイ温度]C</t>
+    <rPh sb="3" eb="5">
+      <t>オンド</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -245,7 +285,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +310,15 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -456,7 +505,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -494,6 +543,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -728,7 +780,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>設定モード</a:t>
+            <a:t>コントラスト設定モード</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1317,33 +1369,30 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="52" name="Shape 51"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="5" idx="4"/>
-          <a:endCxn id="2" idx="2"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1">
-          <a:off x="381000" y="3143250"/>
+          <a:off x="561975" y="4333875"/>
           <a:ext cx="4476750" cy="666750"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector4">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -8510"/>
+            <a:gd name="adj1" fmla="val -7234"/>
             <a:gd name="adj2" fmla="val 347143"/>
           </a:avLst>
         </a:prstGeom>
@@ -1481,15 +1530,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>145840</xdr:rowOff>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1498,13 +1547,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4953000" y="5530850"/>
-          <a:ext cx="1143000" cy="710990"/>
+          <a:off x="3857625" y="7037294"/>
+          <a:ext cx="1143000" cy="1008530"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeEllipseCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -55539"/>
-            <a:gd name="adj2" fmla="val 66694"/>
+            <a:gd name="adj1" fmla="val -60441"/>
+            <a:gd name="adj2" fmla="val 43361"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -1529,7 +1578,26 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>電源電圧表示</a:t>
+            <a:t>電源電圧</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ダイ温度</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>表示</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1565,6 +1633,165 @@
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
             <a:gd name="adj1" fmla="val -389520"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Oval 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2486025" y="7762875"/>
+          <a:ext cx="1333500" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>状態表示モード</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Arrow Connector 26"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="4"/>
+          <a:endCxn id="22" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3143250" y="6858000"/>
+          <a:ext cx="9525" cy="904875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Shape 44"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="22" idx="2"/>
+          <a:endCxn id="2" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="2476501" y="2381251"/>
+          <a:ext cx="9525" cy="5857875"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 21205896"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1876,10 +2103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:AJ38"/>
+  <dimension ref="B2:AJ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="15" customHeight="1"/>
@@ -1889,12 +2116,12 @@
   <sheetData>
     <row r="2" spans="2:34" ht="15" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:34" ht="15" customHeight="1">
       <c r="B3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:34" ht="15" customHeight="1">
@@ -1907,7 +2134,7 @@
     </row>
     <row r="12" spans="2:34" ht="15" customHeight="1">
       <c r="C12" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="3:36" ht="15" customHeight="1">
@@ -1926,32 +2153,35 @@
         <v>8</v>
       </c>
       <c r="AB18" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="3:36" ht="15" customHeight="1">
-      <c r="AG21" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ21" t="s">
-        <v>12</v>
+      <c r="AG21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ21" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="3:36" ht="15" customHeight="1">
       <c r="X22" t="s">
         <v>6</v>
       </c>
-      <c r="AG22" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ22" t="s">
-        <v>13</v>
+      <c r="AG22" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ22" s="13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="3:36" ht="15" customHeight="1">
       <c r="C23" t="s">
         <v>0</v>
       </c>
+      <c r="AG23" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="28" spans="3:36" ht="15" customHeight="1">
       <c r="P28" t="s">
@@ -1960,7 +2190,7 @@
     </row>
     <row r="30" spans="3:36" ht="15" customHeight="1" thickBot="1">
       <c r="AD30" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="3:36" ht="15" customHeight="1">
@@ -1974,7 +2204,7 @@
         <v>3</v>
       </c>
       <c r="AG31" s="6" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="3:36" ht="15" customHeight="1">
@@ -1988,7 +2218,7 @@
         <v>6</v>
       </c>
       <c r="AG32" s="8" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="3:33" ht="15" customHeight="1">
@@ -2002,7 +2232,7 @@
         <v>9</v>
       </c>
       <c r="AG33" s="8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="3:33" ht="15" customHeight="1" thickBot="1">
@@ -2010,21 +2240,29 @@
         <v>1</v>
       </c>
       <c r="AD34" s="9" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AE34" s="10">
         <v>0</v>
       </c>
       <c r="AF34" s="10" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="AG34" s="11" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="3:33" ht="15" customHeight="1">
       <c r="H38" t="s">
-        <v>9</v>
+        <v>26</v>
+      </c>
+      <c r="R38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="3:33" ht="15" customHeight="1">
+      <c r="H41" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2037,10 +2275,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:B17"/>
+  <dimension ref="B2:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2052,62 +2290,75 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="14.25" thickBot="1">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="14.25" thickBot="1">
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="14.25" thickBot="1">
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="12" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="14.25" thickBot="1">
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="14.25" thickBot="1">
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="12" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="14.25" thickBot="1">
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>25</v>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="17" spans="2:2" ht="14.25" thickBot="1">
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="14.25" thickBot="1">
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>